<commit_message>
analisis y datos slang
</commit_message>
<xml_diff>
--- a/data/raw/Drugs.xlsx
+++ b/data/raw/Drugs.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albacortes\Desktop\UPM\TFG\TFG\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2795CBBB-8E27-4D8C-905B-B694EEDB5AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1993E24C-D78A-4222-907B-1E7B51C03658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{20E1C3B8-4C1D-44BF-A8FA-3BA5F597D8F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{20E1C3B8-4C1D-44BF-A8FA-3BA5F597D8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="drug_keyword" sheetId="1" r:id="rId1"/>
     <sheet name="drug" sheetId="2" r:id="rId2"/>
     <sheet name="slang" sheetId="3" r:id="rId3"/>
-    <sheet name="metamap" sheetId="4" r:id="rId4"/>
+    <sheet name="match_slang" sheetId="5" r:id="rId4"/>
+    <sheet name="metamap" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="758">
   <si>
     <t>id</t>
   </si>
@@ -2181,6 +2182,138 @@
   </si>
   <si>
     <t>["sleep"]</t>
+  </si>
+  <si>
+    <t>annotation1</t>
+  </si>
+  <si>
+    <t>annotation2</t>
+  </si>
+  <si>
+    <t>annotation3</t>
+  </si>
+  <si>
+    <t>neutro</t>
+  </si>
+  <si>
+    <t>enegativopuddle</t>
+  </si>
+  <si>
+    <t>enegativotard</t>
+  </si>
+  <si>
+    <t>anxious</t>
+  </si>
+  <si>
+    <t>blotting paper</t>
+  </si>
+  <si>
+    <t>chemicals</t>
+  </si>
+  <si>
+    <t>chewed</t>
+  </si>
+  <si>
+    <t>chewing</t>
+  </si>
+  <si>
+    <t>consuming</t>
+  </si>
+  <si>
+    <t>depressed</t>
+  </si>
+  <si>
+    <t>depressive</t>
+  </si>
+  <si>
+    <t>deshinibition</t>
+  </si>
+  <si>
+    <t>drop in blod pressure</t>
+  </si>
+  <si>
+    <t>drugs</t>
+  </si>
+  <si>
+    <t>flipping</t>
+  </si>
+  <si>
+    <t>improved communication</t>
+  </si>
+  <si>
+    <t>ingested</t>
+  </si>
+  <si>
+    <t>ingesting</t>
+  </si>
+  <si>
+    <t>inhaled</t>
+  </si>
+  <si>
+    <t>inhaling</t>
+  </si>
+  <si>
+    <t>injected</t>
+  </si>
+  <si>
+    <t>injecting</t>
+  </si>
+  <si>
+    <t>lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">music-drug conection </t>
+  </si>
+  <si>
+    <t>paranoid</t>
+  </si>
+  <si>
+    <t>pills</t>
+  </si>
+  <si>
+    <t>raving</t>
+  </si>
+  <si>
+    <t>rolling</t>
+  </si>
+  <si>
+    <t>sexual difficult</t>
+  </si>
+  <si>
+    <t>smoked</t>
+  </si>
+  <si>
+    <t>smoking</t>
+  </si>
+  <si>
+    <t>snorted</t>
+  </si>
+  <si>
+    <t>snorting</t>
+  </si>
+  <si>
+    <t>substances</t>
+  </si>
+  <si>
+    <t>taking</t>
+  </si>
+  <si>
+    <t>vaped</t>
+  </si>
+  <si>
+    <t>vaping</t>
+  </si>
+  <si>
+    <t>vaporized</t>
+  </si>
+  <si>
+    <t>vaporizing</t>
+  </si>
+  <si>
+    <t>vomited</t>
+  </si>
+  <si>
+    <t>vomiting</t>
   </si>
 </sst>
 </file>
@@ -2233,7 +2366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2248,6 +2381,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3179,14 +3315,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A68738-DF46-4C50-94F7-5A6A15D91A39}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -3196,11 +3333,15 @@
       <c r="B1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="C1" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -3212,8 +3353,12 @@
       <c r="C2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -3225,8 +3370,12 @@
       <c r="C3" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -3238,8 +3387,12 @@
       <c r="C4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -3251,8 +3404,12 @@
       <c r="C5" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -3264,8 +3421,12 @@
       <c r="C6" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -3277,8 +3438,12 @@
       <c r="C7" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -3290,8 +3455,12 @@
       <c r="C8" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -3303,8 +3472,12 @@
       <c r="C9" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -3316,8 +3489,12 @@
       <c r="C10" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -3329,8 +3506,12 @@
       <c r="C11" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -3342,8 +3523,12 @@
       <c r="C12" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -3355,8 +3540,12 @@
       <c r="C13" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -3368,8 +3557,12 @@
       <c r="C14" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -3381,8 +3574,12 @@
       <c r="C15" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -3394,8 +3591,12 @@
       <c r="C16" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -3407,8 +3608,12 @@
       <c r="C17" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -3420,8 +3625,12 @@
       <c r="C18" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -3433,8 +3642,12 @@
       <c r="C19" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -3446,8 +3659,12 @@
       <c r="C20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -3459,8 +3676,12 @@
       <c r="C21" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -3472,8 +3693,12 @@
       <c r="C22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -3485,34 +3710,46 @@
       <c r="C23" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>75</v>
+        <v>718</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>719</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -3524,8 +3761,12 @@
       <c r="C26" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -3537,8 +3778,12 @@
       <c r="C27" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -3550,8 +3795,12 @@
       <c r="C28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -3563,8 +3812,12 @@
       <c r="C29" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -3576,8 +3829,12 @@
       <c r="C30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
@@ -3589,8 +3846,12 @@
       <c r="C31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
@@ -3602,8 +3863,12 @@
       <c r="C32" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
@@ -3613,10 +3878,14 @@
         <v>84</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
@@ -3628,8 +3897,12 @@
       <c r="C34" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
@@ -3641,8 +3914,12 @@
       <c r="C35" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
@@ -3654,8 +3931,12 @@
       <c r="C36" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
@@ -3667,8 +3948,12 @@
       <c r="C37" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
@@ -3680,8 +3965,12 @@
       <c r="C38" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
@@ -3693,8 +3982,12 @@
       <c r="C39" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
@@ -3706,8 +3999,12 @@
       <c r="C40" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
@@ -3719,8 +4016,12 @@
       <c r="C41" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
@@ -3732,8 +4033,12 @@
       <c r="C42" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
@@ -3743,10 +4048,14 @@
         <v>94</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
@@ -3758,8 +4067,12 @@
       <c r="C44" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
@@ -3771,8 +4084,12 @@
       <c r="C45" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
@@ -3784,8 +4101,12 @@
       <c r="C46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
@@ -3797,8 +4118,12 @@
       <c r="C47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
@@ -3810,8 +4135,12 @@
       <c r="C48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
@@ -3823,8 +4152,12 @@
       <c r="C49" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
@@ -3836,8 +4169,12 @@
       <c r="C50" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
@@ -3849,8 +4186,12 @@
       <c r="C51" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
@@ -3862,8 +4203,12 @@
       <c r="C52" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="D52" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
@@ -3875,8 +4220,12 @@
       <c r="C53" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
@@ -3888,8 +4237,12 @@
       <c r="C54" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
@@ -3899,10 +4252,14 @@
         <v>106</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
@@ -3914,8 +4271,12 @@
       <c r="C56" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
@@ -3927,8 +4288,12 @@
       <c r="C57" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="D57" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
@@ -3940,8 +4305,12 @@
       <c r="C58" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
@@ -3953,8 +4322,12 @@
       <c r="C59" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
@@ -3966,8 +4339,12 @@
       <c r="C60" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
@@ -3979,8 +4356,12 @@
       <c r="C61" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
+      <c r="D61" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
@@ -3992,8 +4373,12 @@
       <c r="C62" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
+      <c r="D62" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
@@ -4005,8 +4390,12 @@
       <c r="C63" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
+      <c r="D63" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
@@ -4018,8 +4407,12 @@
       <c r="C64" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
+      <c r="D64" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
@@ -4031,8 +4424,12 @@
       <c r="C65" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
@@ -4044,8 +4441,12 @@
       <c r="C66" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
@@ -4057,8 +4458,12 @@
       <c r="C67" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
+      <c r="D67" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
@@ -4070,8 +4475,12 @@
       <c r="C68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
@@ -4081,10 +4490,14 @@
         <v>120</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
@@ -4096,8 +4509,12 @@
       <c r="C70" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
@@ -4109,8 +4526,12 @@
       <c r="C71" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
+      <c r="D71" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
@@ -4122,8 +4543,12 @@
       <c r="C72" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
+      <c r="D72" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
@@ -4135,8 +4560,12 @@
       <c r="C73" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
+      <c r="D73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
@@ -4148,8 +4577,12 @@
       <c r="C74" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
+      <c r="D74" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
@@ -4161,8 +4594,12 @@
       <c r="C75" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
@@ -4174,8 +4611,12 @@
       <c r="C76" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
@@ -4187,8 +4628,12 @@
       <c r="C77" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
+      <c r="D77" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
@@ -4200,8 +4645,12 @@
       <c r="C78" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
+      <c r="D78" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
@@ -4213,8 +4662,12 @@
       <c r="C79" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
+      <c r="D79" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
@@ -4224,10 +4677,14 @@
         <v>131</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
@@ -4239,8 +4696,12 @@
       <c r="C81" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
+      <c r="D81" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
@@ -4252,8 +4713,12 @@
       <c r="C82" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
+      <c r="D82" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
@@ -4265,8 +4730,12 @@
       <c r="C83" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
@@ -4278,8 +4747,12 @@
       <c r="C84" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
+      <c r="D84" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
@@ -4291,8 +4764,12 @@
       <c r="C85" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
+      <c r="D85" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
@@ -4304,8 +4781,12 @@
       <c r="C86" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
@@ -4317,8 +4798,12 @@
       <c r="C87" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
+      <c r="D87" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
@@ -4330,8 +4815,12 @@
       <c r="C88" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
+      <c r="D88" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
@@ -4341,10 +4830,14 @@
         <v>140</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
@@ -4356,8 +4849,12 @@
       <c r="C90" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
+      <c r="D90" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4365,6 +4862,1045 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ABE646-4DE9-48C4-A104-AD51B63E37A6}">
+  <dimension ref="A1:B128"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B128"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>26</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>31</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>31</v>
+      </c>
+      <c r="B42" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>33</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>35</v>
+      </c>
+      <c r="B46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>37</v>
+      </c>
+      <c r="B48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>38</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>40</v>
+      </c>
+      <c r="B52" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>40</v>
+      </c>
+      <c r="B53" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>41</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>41</v>
+      </c>
+      <c r="B55" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>41</v>
+      </c>
+      <c r="B56" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>42</v>
+      </c>
+      <c r="B57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>42</v>
+      </c>
+      <c r="B58" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>42</v>
+      </c>
+      <c r="B59" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>43</v>
+      </c>
+      <c r="B60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>44</v>
+      </c>
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>45</v>
+      </c>
+      <c r="B62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>46</v>
+      </c>
+      <c r="B63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>47</v>
+      </c>
+      <c r="B64" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>48</v>
+      </c>
+      <c r="B65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>48</v>
+      </c>
+      <c r="B66" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>49</v>
+      </c>
+      <c r="B67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>50</v>
+      </c>
+      <c r="B68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>51</v>
+      </c>
+      <c r="B69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>52</v>
+      </c>
+      <c r="B70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>53</v>
+      </c>
+      <c r="B71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>54</v>
+      </c>
+      <c r="B72" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>55</v>
+      </c>
+      <c r="B73" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>56</v>
+      </c>
+      <c r="B74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>57</v>
+      </c>
+      <c r="B75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>58</v>
+      </c>
+      <c r="B76" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>59</v>
+      </c>
+      <c r="B77" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>61</v>
+      </c>
+      <c r="B79" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>61</v>
+      </c>
+      <c r="B80" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>62</v>
+      </c>
+      <c r="B81" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>63</v>
+      </c>
+      <c r="B82" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>63</v>
+      </c>
+      <c r="B83" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>64</v>
+      </c>
+      <c r="B84" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>65</v>
+      </c>
+      <c r="B85" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>66</v>
+      </c>
+      <c r="B86" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>66</v>
+      </c>
+      <c r="B87" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>67</v>
+      </c>
+      <c r="B88" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>68</v>
+      </c>
+      <c r="B89" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>68</v>
+      </c>
+      <c r="B90" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>69</v>
+      </c>
+      <c r="B91" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>70</v>
+      </c>
+      <c r="B92" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>71</v>
+      </c>
+      <c r="B93" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>72</v>
+      </c>
+      <c r="B94" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>73</v>
+      </c>
+      <c r="B95" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>74</v>
+      </c>
+      <c r="B96" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>74</v>
+      </c>
+      <c r="B97" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>74</v>
+      </c>
+      <c r="B98" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>75</v>
+      </c>
+      <c r="B99" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>75</v>
+      </c>
+      <c r="B100" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>75</v>
+      </c>
+      <c r="B101" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>76</v>
+      </c>
+      <c r="B102" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>77</v>
+      </c>
+      <c r="B103" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>78</v>
+      </c>
+      <c r="B104" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>79</v>
+      </c>
+      <c r="B105" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>79</v>
+      </c>
+      <c r="B106" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>80</v>
+      </c>
+      <c r="B107" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>81</v>
+      </c>
+      <c r="B108" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>82</v>
+      </c>
+      <c r="B109" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>82</v>
+      </c>
+      <c r="B110" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>83</v>
+      </c>
+      <c r="B111" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>84</v>
+      </c>
+      <c r="B112" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>85</v>
+      </c>
+      <c r="B113" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>86</v>
+      </c>
+      <c r="B114" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>86</v>
+      </c>
+      <c r="B115" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>86</v>
+      </c>
+      <c r="B116" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>87</v>
+      </c>
+      <c r="B117" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>87</v>
+      </c>
+      <c r="B118" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>87</v>
+      </c>
+      <c r="B119" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>88</v>
+      </c>
+      <c r="B120" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>88</v>
+      </c>
+      <c r="B121" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>88</v>
+      </c>
+      <c r="B122" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>89</v>
+      </c>
+      <c r="B123" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>90</v>
+      </c>
+      <c r="B124" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>91</v>
+      </c>
+      <c r="B125" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>92</v>
+      </c>
+      <c r="B126" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>93</v>
+      </c>
+      <c r="B127" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>94</v>
+      </c>
+      <c r="B128" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F6F4E2-8F0D-419A-B5E4-8235A9D0F903}">
   <dimension ref="A1:E286"/>
   <sheetViews>
@@ -9247,6 +10783,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e272a2e4-4bdf-4402-86c1-14e941d15658" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EB04A42EC1A26F4FBB63D166FC5B970D" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="239dad6c5680f2618a3beaced7d7cca6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e272a2e4-4bdf-4402-86c1-14e941d15658" xmlns:ns4="d4db9376-2a30-4459-9193-cfeb797d1955" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ecfe34017f2e154931bc78fb9fcd0a2" ns3:_="" ns4:_="">
     <xsd:import namespace="e272a2e4-4bdf-4402-86c1-14e941d15658"/>
@@ -9499,38 +11052,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e272a2e4-4bdf-4402-86c1-14e941d15658" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89FDF4BC-CCAE-4FF5-92C8-A45E4D33E3D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B5AAE4-66A7-4C08-B099-49C1C4975ADD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e272a2e4-4bdf-4402-86c1-14e941d15658"/>
-    <ds:schemaRef ds:uri="d4db9376-2a30-4459-9193-cfeb797d1955"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9553,9 +11078,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B5AAE4-66A7-4C08-B099-49C1C4975ADD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89FDF4BC-CCAE-4FF5-92C8-A45E4D33E3D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e272a2e4-4bdf-4402-86c1-14e941d15658"/>
+    <ds:schemaRef ds:uri="d4db9376-2a30-4459-9193-cfeb797d1955"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>